<commit_message>
Large commit bringing git source up to date with darks source and the 0.13 ruby gem.
</commit_message>
<xml_diff>
--- a/examples/sheets/pruning.xlsx
+++ b/examples/sheets/pruning.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20412"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="20760" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="140" yWindow="0" windowWidth="33360" windowHeight="20300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Outputs" sheetId="1" r:id="rId1"/>
@@ -14,9 +14,9 @@
   <definedNames>
     <definedName name="In_result">Inputs!$A$3</definedName>
   </definedNames>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Result</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -48,19 +48,55 @@
   <si>
     <t>Doesn't depend on an input</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Indirect value:</t>
+  </si>
+  <si>
+    <t>Indirect</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Indirect table</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Indirect table 2</t>
+  </si>
+  <si>
+    <t>table1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
     <font>
       <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Verdana"/>
     </font>
   </fonts>
@@ -81,18 +117,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B21:C22" totalsRowShown="0">
+  <autoFilter ref="B21:C22"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="A"/>
+    <tableColumn id="2" name="b">
+      <calculatedColumnFormula>A4</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -414,14 +467,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C15" sqref="C15:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -453,12 +506,45 @@
         <v>Doesn't depend on an input</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <f ca="1">INDIRECT("'Calcs'!a17")</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <f ca="1">INDIRECT(A9&amp;"[B]")</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -466,14 +552,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:D13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1">
@@ -549,13 +635,43 @@
         <v>5</v>
       </c>
     </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <f>A4</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <f>A4</f>
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -563,14 +679,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1">
@@ -588,12 +704,11 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Fix the incorrect pruning of arraying formulas
</commit_message>
<xml_diff>
--- a/examples/sheets/pruning.xlsx
+++ b/examples/sheets/pruning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="0" windowWidth="33360" windowHeight="20300" tabRatio="500"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="In_result">Inputs!$A$3</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" calcMode="manual" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Result</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>table1</t>
+  </si>
+  <si>
+    <t>Arraying formula</t>
   </si>
 </sst>
 </file>
@@ -468,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:D15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -537,6 +540,15 @@
     <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f>Inputs!E6</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -680,27 +692,62 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5">
       <c r="A1">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <f t="array" ref="A6:E6">A5:E5</f>
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>